<commit_message>
changes in excel file and other condition
</commit_message>
<xml_diff>
--- a/purchasedGoods.xlsx
+++ b/purchasedGoods.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Abhishek Projects\Eco Trace\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E545EA0-5FAD-43E6-8571-6654DB72AD6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F34BCE92-943B-4E18-B7BF-3E42E27D50D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Template" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Template!$A$1:$E$158</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Template!$A$1:$F$158</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t>S. No.</t>
   </si>
@@ -81,6 +81,9 @@
   </si>
   <si>
     <t>Vendor Specific</t>
+  </si>
+  <si>
+    <t>Product Category</t>
   </si>
 </sst>
 </file>
@@ -194,7 +197,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -431,183 +434,187 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB998"/>
+  <dimension ref="A1:AC998"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AB1" sqref="AB1:AB1048576"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.42578125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="7.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="15.42578125" style="3" customWidth="1"/>
-    <col min="12" max="13" width="7.7109375" style="3" customWidth="1"/>
-    <col min="14" max="14" width="13.5703125" style="3" customWidth="1"/>
-    <col min="15" max="19" width="7.7109375" style="3" customWidth="1"/>
-    <col min="20" max="20" width="6.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="22" max="26" width="7.7109375" style="3" customWidth="1"/>
-    <col min="27" max="28" width="8" style="3" customWidth="1"/>
+    <col min="2" max="2" width="33.5703125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="23.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.42578125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="7.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="15.42578125" style="3" customWidth="1"/>
+    <col min="13" max="14" width="7.7109375" style="3" customWidth="1"/>
+    <col min="15" max="15" width="13.5703125" style="3" customWidth="1"/>
+    <col min="16" max="20" width="7.7109375" style="3" customWidth="1"/>
+    <col min="21" max="21" width="6.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="23" max="27" width="7.7109375" style="3" customWidth="1"/>
+    <col min="28" max="29" width="8" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="1"/>
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="U1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="V1" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="2" t="str">
-        <f>IF(ISTEXT(E2), VLOOKUP(E2,$T$1:$U$4,2,FALSE),)</f>
+      <c r="J2" s="2" t="str">
+        <f>IF(ISTEXT(F2), VLOOKUP(F2,$U$1:$V$4,2,FALSE),)</f>
         <v>kg CO2e / kg</v>
       </c>
-      <c r="T2" s="3" t="s">
+      <c r="U2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="U2" s="3" t="s">
+      <c r="V2" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <f t="shared" ref="A3:A158" si="0">A2+1</f>
         <v>2</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="2" t="str">
-        <f>IF(ISTEXT(E3), VLOOKUP(E3,$T$1:$U$4,2,FALSE),)</f>
+      <c r="J3" s="2" t="str">
+        <f>IF(ISTEXT(F3), VLOOKUP(F3,$U$1:$V$4,2,FALSE),)</f>
         <v>kg CO2e / Litres</v>
       </c>
-      <c r="T3" s="3" t="s">
+      <c r="U3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="U3" s="3" t="s">
+      <c r="V3" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="2" t="str">
-        <f>IF(ISTEXT(E4), VLOOKUP(E4,$T$1:$U$4,2,FALSE),)</f>
+      <c r="J4" s="2" t="str">
+        <f>IF(ISTEXT(F4), VLOOKUP(F4,$U$1:$V$4,2,FALSE),)</f>
         <v>kg CO2e / Litres</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1381,99 +1388,99 @@
         <v>143</v>
       </c>
     </row>
-    <row r="145" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A145" s="2">
         <f t="shared" si="0"/>
         <v>144</v>
       </c>
     </row>
-    <row r="146" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A146" s="2">
         <f t="shared" si="0"/>
         <v>145</v>
       </c>
     </row>
-    <row r="147" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A147" s="2">
         <f t="shared" si="0"/>
         <v>146</v>
       </c>
     </row>
-    <row r="148" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A148" s="2">
         <f t="shared" si="0"/>
         <v>147</v>
       </c>
     </row>
-    <row r="149" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A149" s="2">
         <f t="shared" si="0"/>
         <v>148</v>
       </c>
     </row>
-    <row r="150" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A150" s="2">
         <f t="shared" si="0"/>
         <v>149</v>
       </c>
     </row>
-    <row r="151" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A151" s="2">
         <f t="shared" si="0"/>
         <v>150</v>
       </c>
     </row>
-    <row r="152" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A152" s="2">
         <f t="shared" si="0"/>
         <v>151</v>
       </c>
     </row>
-    <row r="153" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A153" s="2">
         <f t="shared" si="0"/>
         <v>152</v>
       </c>
     </row>
-    <row r="154" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A154" s="2">
         <f t="shared" si="0"/>
         <v>153</v>
       </c>
     </row>
-    <row r="155" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A155" s="2">
         <f t="shared" si="0"/>
         <v>154</v>
       </c>
     </row>
-    <row r="156" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A156" s="2">
         <f t="shared" si="0"/>
         <v>155</v>
       </c>
     </row>
-    <row r="157" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A157" s="2">
         <f t="shared" si="0"/>
         <v>156</v>
       </c>
     </row>
-    <row r="158" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A158" s="2">
         <f t="shared" si="0"/>
         <v>157</v>
       </c>
     </row>
-    <row r="159" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="160" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C160" s="2">
-        <v>1</v>
-      </c>
+    <row r="159" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="160" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D160" s="2">
         <v>1</v>
       </c>
       <c r="E160" s="2">
+        <v>1</v>
+      </c>
+      <c r="F160" s="2">
         <v>1</v>
       </c>
     </row>
@@ -2316,10 +2323,10 @@
     <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <autoFilter ref="A1:E158" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:F158" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E158" xr:uid="{00000000-0002-0000-0000-000000000000}">
-      <formula1>$T$1:$T$4</formula1>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F2:F158" xr:uid="{00000000-0002-0000-0000-000000000000}">
+      <formula1>$U$1:$U$4</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>

</xml_diff>